<commit_message>
I changed the solution to open the file for viewing
</commit_message>
<xml_diff>
--- a/CardiffWorkNotebook.xlsx
+++ b/CardiffWorkNotebook.xlsx
@@ -457,19 +457,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,11 +849,11 @@
   </sheetPr>
   <dimension ref="A1:CV48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="4.7109375" customWidth="1" min="1" max="1"/>
     <col width="3.28515625" customWidth="1" min="2" max="2"/>
@@ -872,160 +872,160 @@
     <row r="2">
       <c r="A2" s="16" t="n"/>
       <c r="B2" s="18" t="n"/>
-      <c r="C2" s="36" t="inlineStr">
+      <c r="C2" s="32" t="inlineStr">
         <is>
           <t>29 tyg.</t>
         </is>
       </c>
-      <c r="D2" s="37" t="n"/>
-      <c r="E2" s="37" t="n"/>
-      <c r="F2" s="37" t="n"/>
-      <c r="G2" s="37" t="n"/>
-      <c r="H2" s="37" t="n"/>
-      <c r="I2" s="38" t="n"/>
-      <c r="J2" s="36" t="inlineStr">
+      <c r="D2" s="33" t="n"/>
+      <c r="E2" s="33" t="n"/>
+      <c r="F2" s="33" t="n"/>
+      <c r="G2" s="33" t="n"/>
+      <c r="H2" s="33" t="n"/>
+      <c r="I2" s="34" t="n"/>
+      <c r="J2" s="32" t="inlineStr">
         <is>
           <t>30 tyg.</t>
         </is>
       </c>
-      <c r="K2" s="37" t="n"/>
-      <c r="L2" s="37" t="n"/>
-      <c r="M2" s="37" t="n"/>
-      <c r="N2" s="37" t="n"/>
-      <c r="O2" s="37" t="n"/>
-      <c r="P2" s="38" t="n"/>
+      <c r="K2" s="33" t="n"/>
+      <c r="L2" s="33" t="n"/>
+      <c r="M2" s="33" t="n"/>
+      <c r="N2" s="33" t="n"/>
+      <c r="O2" s="33" t="n"/>
+      <c r="P2" s="34" t="n"/>
       <c r="Q2" s="41" t="inlineStr">
         <is>
           <t>31 tyg.</t>
         </is>
       </c>
-      <c r="R2" s="37" t="n"/>
-      <c r="S2" s="37" t="n"/>
-      <c r="T2" s="37" t="n"/>
-      <c r="U2" s="37" t="n"/>
-      <c r="V2" s="37" t="n"/>
-      <c r="W2" s="37" t="n"/>
-      <c r="X2" s="36" t="inlineStr">
+      <c r="R2" s="33" t="n"/>
+      <c r="S2" s="33" t="n"/>
+      <c r="T2" s="33" t="n"/>
+      <c r="U2" s="33" t="n"/>
+      <c r="V2" s="33" t="n"/>
+      <c r="W2" s="33" t="n"/>
+      <c r="X2" s="32" t="inlineStr">
         <is>
           <t>32 tyg.</t>
         </is>
       </c>
-      <c r="Y2" s="37" t="n"/>
-      <c r="Z2" s="37" t="n"/>
-      <c r="AA2" s="37" t="n"/>
-      <c r="AB2" s="37" t="n"/>
-      <c r="AC2" s="37" t="n"/>
-      <c r="AD2" s="38" t="n"/>
-      <c r="AE2" s="36" t="inlineStr">
+      <c r="Y2" s="33" t="n"/>
+      <c r="Z2" s="33" t="n"/>
+      <c r="AA2" s="33" t="n"/>
+      <c r="AB2" s="33" t="n"/>
+      <c r="AC2" s="33" t="n"/>
+      <c r="AD2" s="34" t="n"/>
+      <c r="AE2" s="32" t="inlineStr">
         <is>
           <t>33 tyg.</t>
         </is>
       </c>
-      <c r="AF2" s="37" t="n"/>
-      <c r="AG2" s="37" t="n"/>
-      <c r="AH2" s="37" t="n"/>
-      <c r="AI2" s="37" t="n"/>
-      <c r="AJ2" s="37" t="n"/>
-      <c r="AK2" s="38" t="n"/>
-      <c r="AL2" s="36" t="inlineStr">
+      <c r="AF2" s="33" t="n"/>
+      <c r="AG2" s="33" t="n"/>
+      <c r="AH2" s="33" t="n"/>
+      <c r="AI2" s="33" t="n"/>
+      <c r="AJ2" s="33" t="n"/>
+      <c r="AK2" s="34" t="n"/>
+      <c r="AL2" s="32" t="inlineStr">
         <is>
           <t>34 tyg.</t>
         </is>
       </c>
-      <c r="AM2" s="37" t="n"/>
-      <c r="AN2" s="37" t="n"/>
-      <c r="AO2" s="37" t="n"/>
-      <c r="AP2" s="37" t="n"/>
-      <c r="AQ2" s="37" t="n"/>
-      <c r="AR2" s="38" t="n"/>
-      <c r="AS2" s="36" t="inlineStr">
+      <c r="AM2" s="33" t="n"/>
+      <c r="AN2" s="33" t="n"/>
+      <c r="AO2" s="33" t="n"/>
+      <c r="AP2" s="33" t="n"/>
+      <c r="AQ2" s="33" t="n"/>
+      <c r="AR2" s="34" t="n"/>
+      <c r="AS2" s="32" t="inlineStr">
         <is>
           <t>35 tyg.</t>
         </is>
       </c>
-      <c r="AT2" s="37" t="n"/>
-      <c r="AU2" s="37" t="n"/>
-      <c r="AV2" s="37" t="n"/>
-      <c r="AW2" s="37" t="n"/>
-      <c r="AX2" s="37" t="n"/>
-      <c r="AY2" s="38" t="n"/>
-      <c r="AZ2" s="36" t="inlineStr">
+      <c r="AT2" s="33" t="n"/>
+      <c r="AU2" s="33" t="n"/>
+      <c r="AV2" s="33" t="n"/>
+      <c r="AW2" s="33" t="n"/>
+      <c r="AX2" s="33" t="n"/>
+      <c r="AY2" s="34" t="n"/>
+      <c r="AZ2" s="32" t="inlineStr">
         <is>
           <t>36 tyg.</t>
         </is>
       </c>
-      <c r="BA2" s="37" t="n"/>
-      <c r="BB2" s="37" t="n"/>
-      <c r="BC2" s="37" t="n"/>
-      <c r="BD2" s="37" t="n"/>
-      <c r="BE2" s="37" t="n"/>
-      <c r="BF2" s="38" t="n"/>
-      <c r="BG2" s="36" t="inlineStr">
+      <c r="BA2" s="33" t="n"/>
+      <c r="BB2" s="33" t="n"/>
+      <c r="BC2" s="33" t="n"/>
+      <c r="BD2" s="33" t="n"/>
+      <c r="BE2" s="33" t="n"/>
+      <c r="BF2" s="34" t="n"/>
+      <c r="BG2" s="32" t="inlineStr">
         <is>
           <t>37 tyg.</t>
         </is>
       </c>
-      <c r="BH2" s="37" t="n"/>
-      <c r="BI2" s="37" t="n"/>
-      <c r="BJ2" s="37" t="n"/>
-      <c r="BK2" s="37" t="n"/>
-      <c r="BL2" s="37" t="n"/>
-      <c r="BM2" s="38" t="n"/>
-      <c r="BN2" s="36" t="inlineStr">
+      <c r="BH2" s="33" t="n"/>
+      <c r="BI2" s="33" t="n"/>
+      <c r="BJ2" s="33" t="n"/>
+      <c r="BK2" s="33" t="n"/>
+      <c r="BL2" s="33" t="n"/>
+      <c r="BM2" s="34" t="n"/>
+      <c r="BN2" s="32" t="inlineStr">
         <is>
           <t>38 tyg.</t>
         </is>
       </c>
-      <c r="BO2" s="37" t="n"/>
-      <c r="BP2" s="37" t="n"/>
-      <c r="BQ2" s="37" t="n"/>
-      <c r="BR2" s="37" t="n"/>
-      <c r="BS2" s="37" t="n"/>
-      <c r="BT2" s="38" t="n"/>
-      <c r="BU2" s="36" t="inlineStr">
+      <c r="BO2" s="33" t="n"/>
+      <c r="BP2" s="33" t="n"/>
+      <c r="BQ2" s="33" t="n"/>
+      <c r="BR2" s="33" t="n"/>
+      <c r="BS2" s="33" t="n"/>
+      <c r="BT2" s="34" t="n"/>
+      <c r="BU2" s="32" t="inlineStr">
         <is>
           <t>39 tyg.</t>
         </is>
       </c>
-      <c r="BV2" s="37" t="n"/>
-      <c r="BW2" s="37" t="n"/>
-      <c r="BX2" s="37" t="n"/>
-      <c r="BY2" s="37" t="n"/>
-      <c r="BZ2" s="37" t="n"/>
-      <c r="CA2" s="38" t="n"/>
-      <c r="CB2" s="36" t="inlineStr">
+      <c r="BV2" s="33" t="n"/>
+      <c r="BW2" s="33" t="n"/>
+      <c r="BX2" s="33" t="n"/>
+      <c r="BY2" s="33" t="n"/>
+      <c r="BZ2" s="33" t="n"/>
+      <c r="CA2" s="34" t="n"/>
+      <c r="CB2" s="32" t="inlineStr">
         <is>
           <t>40 tyg.</t>
         </is>
       </c>
-      <c r="CC2" s="37" t="n"/>
-      <c r="CD2" s="37" t="n"/>
-      <c r="CE2" s="37" t="n"/>
-      <c r="CF2" s="37" t="n"/>
-      <c r="CG2" s="37" t="n"/>
-      <c r="CH2" s="38" t="n"/>
-      <c r="CI2" s="36" t="inlineStr">
+      <c r="CC2" s="33" t="n"/>
+      <c r="CD2" s="33" t="n"/>
+      <c r="CE2" s="33" t="n"/>
+      <c r="CF2" s="33" t="n"/>
+      <c r="CG2" s="33" t="n"/>
+      <c r="CH2" s="34" t="n"/>
+      <c r="CI2" s="32" t="inlineStr">
         <is>
           <t>41 tyg.</t>
         </is>
       </c>
-      <c r="CJ2" s="37" t="n"/>
-      <c r="CK2" s="37" t="n"/>
-      <c r="CL2" s="37" t="n"/>
-      <c r="CM2" s="37" t="n"/>
-      <c r="CN2" s="37" t="n"/>
-      <c r="CO2" s="38" t="n"/>
-      <c r="CP2" s="36" t="inlineStr">
+      <c r="CJ2" s="33" t="n"/>
+      <c r="CK2" s="33" t="n"/>
+      <c r="CL2" s="33" t="n"/>
+      <c r="CM2" s="33" t="n"/>
+      <c r="CN2" s="33" t="n"/>
+      <c r="CO2" s="34" t="n"/>
+      <c r="CP2" s="32" t="inlineStr">
         <is>
           <t>42 tyg.</t>
         </is>
       </c>
-      <c r="CQ2" s="37" t="n"/>
-      <c r="CR2" s="37" t="n"/>
-      <c r="CS2" s="37" t="n"/>
-      <c r="CT2" s="37" t="n"/>
-      <c r="CU2" s="37" t="n"/>
-      <c r="CV2" s="38" t="n"/>
+      <c r="CQ2" s="33" t="n"/>
+      <c r="CR2" s="33" t="n"/>
+      <c r="CS2" s="33" t="n"/>
+      <c r="CT2" s="33" t="n"/>
+      <c r="CU2" s="33" t="n"/>
+      <c r="CV2" s="34" t="n"/>
     </row>
     <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="28" t="n">
@@ -1545,8 +1545,16 @@
       <c r="Q4" s="2" t="n"/>
       <c r="R4" s="4" t="n"/>
       <c r="S4" s="4" t="n"/>
-      <c r="T4" s="4" t="n"/>
-      <c r="U4" s="4" t="n"/>
+      <c r="T4" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U4" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V4" s="4" t="n"/>
       <c r="W4" s="4" t="n"/>
       <c r="X4" s="2" t="n"/>
@@ -1634,22 +1642,66 @@
       <c r="B5" s="21" t="n"/>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="4" t="n"/>
-      <c r="E5" s="4" t="n"/>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="n"/>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" s="4" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="2" t="n"/>
-      <c r="K5" s="4" t="n"/>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="4" t="n"/>
-      <c r="N5" s="4" t="n"/>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O5" s="4" t="n"/>
-      <c r="P5" s="3" t="n"/>
+      <c r="P5" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q5" s="2" t="n"/>
       <c r="R5" s="4" t="n"/>
-      <c r="S5" s="4" t="n"/>
-      <c r="T5" s="4" t="n"/>
+      <c r="S5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T5" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U5" s="4" t="n"/>
       <c r="V5" s="4" t="n"/>
       <c r="W5" s="4" t="n"/>
@@ -1744,21 +1796,45 @@
       <c r="H6" s="4" t="n"/>
       <c r="I6" s="3" t="n"/>
       <c r="J6" s="2" t="n"/>
-      <c r="K6" s="4" t="n"/>
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L6" s="4" t="n"/>
-      <c r="M6" s="4" t="n"/>
-      <c r="N6" s="4" t="n"/>
+      <c r="M6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O6" s="4" t="n"/>
       <c r="P6" s="3" t="n"/>
-      <c r="Q6" s="2" t="n"/>
-      <c r="R6" s="4" t="n"/>
-      <c r="S6" s="4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T6" s="4" t="n"/>
-      <c r="U6" s="4" t="n"/>
+      <c r="Q6" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S6" s="4" t="n"/>
+      <c r="T6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U6" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V6" s="4" t="n"/>
       <c r="W6" s="4" t="n"/>
       <c r="X6" s="2" t="n"/>
@@ -1847,23 +1923,67 @@
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="4" t="n"/>
       <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="4" t="n"/>
-      <c r="I7" s="3" t="n"/>
-      <c r="J7" s="2" t="n"/>
-      <c r="K7" s="4" t="n"/>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="4" t="n"/>
       <c r="N7" s="4" t="n"/>
-      <c r="O7" s="4" t="n"/>
-      <c r="P7" s="3" t="n"/>
-      <c r="Q7" s="2" t="n"/>
-      <c r="R7" s="4" t="n"/>
-      <c r="S7" s="4" t="n"/>
+      <c r="O7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P7" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q7" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T7" s="4" t="n"/>
       <c r="U7" s="4" t="n"/>
-      <c r="V7" s="4" t="n"/>
+      <c r="V7" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W7" s="4" t="n"/>
       <c r="X7" s="2" t="n"/>
       <c r="Y7" s="4" t="n"/>
@@ -1950,23 +2070,67 @@
       </c>
       <c r="C8" s="4" t="n"/>
       <c r="D8" s="4" t="n"/>
-      <c r="E8" s="4" t="n"/>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H8" s="4" t="n"/>
       <c r="I8" s="3" t="n"/>
-      <c r="J8" s="2" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="4" t="n"/>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M8" s="4" t="n"/>
       <c r="N8" s="4" t="n"/>
-      <c r="O8" s="4" t="n"/>
-      <c r="P8" s="3" t="n"/>
-      <c r="Q8" s="2" t="n"/>
-      <c r="R8" s="4" t="n"/>
+      <c r="O8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q8" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S8" s="4" t="n"/>
-      <c r="T8" s="4" t="n"/>
-      <c r="U8" s="4" t="n"/>
+      <c r="T8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U8" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V8" s="4" t="n"/>
       <c r="W8" s="4" t="n"/>
       <c r="X8" s="2" t="n"/>
@@ -2054,23 +2218,59 @@
       <c r="B9" s="21" t="n"/>
       <c r="C9" s="4" t="n"/>
       <c r="D9" s="4" t="n"/>
-      <c r="E9" s="4" t="n"/>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="3" t="n"/>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J9" s="2" t="n"/>
       <c r="K9" s="4" t="n"/>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
+      <c r="L9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N9" s="4" t="n"/>
       <c r="O9" s="4" t="n"/>
       <c r="P9" s="3" t="n"/>
-      <c r="Q9" s="2" t="n"/>
-      <c r="R9" s="4" t="n"/>
+      <c r="Q9" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S9" s="4" t="n"/>
       <c r="T9" s="4" t="n"/>
-      <c r="U9" s="4" t="n"/>
+      <c r="U9" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V9" s="4" t="n"/>
       <c r="W9" s="4" t="n"/>
       <c r="X9" s="2" t="n"/>
@@ -2159,20 +2359,56 @@
       <c r="C10" s="4" t="n"/>
       <c r="D10" s="4" t="n"/>
       <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H10" s="4" t="n"/>
       <c r="I10" s="3" t="n"/>
-      <c r="J10" s="2" t="n"/>
-      <c r="K10" s="4" t="n"/>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L10" s="4" t="n"/>
-      <c r="M10" s="4" t="n"/>
-      <c r="N10" s="4" t="n"/>
-      <c r="O10" s="4" t="n"/>
-      <c r="P10" s="3" t="n"/>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P10" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q10" s="2" t="n"/>
       <c r="R10" s="4" t="n"/>
-      <c r="S10" s="4" t="n"/>
+      <c r="S10" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T10" s="4" t="n"/>
       <c r="U10" s="4" t="n"/>
       <c r="V10" s="4" t="n"/>
@@ -2264,22 +2500,50 @@
       <c r="D11" s="4" t="n"/>
       <c r="E11" s="4" t="n"/>
       <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="4" t="n"/>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I11" s="3" t="n"/>
-      <c r="J11" s="2" t="n"/>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K11" s="4" t="n"/>
       <c r="L11" s="4" t="n"/>
-      <c r="M11" s="4" t="n"/>
+      <c r="M11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N11" s="4" t="n"/>
-      <c r="O11" s="4" t="n"/>
+      <c r="O11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P11" s="3" t="n"/>
       <c r="Q11" s="2" t="n"/>
       <c r="R11" s="4" t="n"/>
-      <c r="S11" s="4" t="n"/>
+      <c r="S11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T11" s="4" t="n"/>
       <c r="U11" s="4" t="n"/>
-      <c r="V11" s="4" t="n"/>
+      <c r="V11" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W11" s="4" t="n"/>
       <c r="X11" s="2" t="n"/>
       <c r="Y11" s="4" t="n"/>
@@ -2367,22 +2631,74 @@
       <c r="C12" s="4" t="n"/>
       <c r="D12" s="4" t="n"/>
       <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="3" t="n"/>
-      <c r="J12" s="2" t="n"/>
+      <c r="H12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-      <c r="O12" s="4" t="n"/>
-      <c r="P12" s="3" t="n"/>
-      <c r="Q12" s="2" t="n"/>
-      <c r="R12" s="4" t="n"/>
-      <c r="S12" s="4" t="n"/>
+      <c r="L12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P12" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q12" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T12" s="4" t="n"/>
-      <c r="U12" s="4" t="n"/>
+      <c r="U12" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V12" s="4" t="n"/>
       <c r="W12" s="4" t="n"/>
       <c r="X12" s="2" t="n"/>
@@ -2470,24 +2786,60 @@
       <c r="B13" s="21" t="n"/>
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H13" s="4" t="n"/>
       <c r="I13" s="3" t="n"/>
-      <c r="J13" s="2" t="n"/>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K13" s="4" t="n"/>
       <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-      <c r="O13" s="4" t="n"/>
-      <c r="P13" s="3" t="n"/>
+      <c r="M13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P13" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q13" s="2" t="n"/>
       <c r="R13" s="4" t="n"/>
       <c r="S13" s="4" t="n"/>
-      <c r="T13" s="4" t="n"/>
+      <c r="T13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U13" s="4" t="n"/>
-      <c r="V13" s="4" t="n"/>
+      <c r="V13" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W13" s="4" t="n"/>
       <c r="X13" s="2" t="n"/>
       <c r="Y13" s="4" t="n"/>
@@ -2574,23 +2926,63 @@
       </c>
       <c r="C14" s="4" t="n"/>
       <c r="D14" s="4" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="3" t="n"/>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J14" s="2" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
-      <c r="M14" s="4" t="n"/>
+      <c r="K14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N14" s="4" t="n"/>
       <c r="O14" s="4" t="n"/>
       <c r="P14" s="3" t="n"/>
       <c r="Q14" s="2" t="n"/>
       <c r="R14" s="4" t="n"/>
       <c r="S14" s="4" t="n"/>
-      <c r="T14" s="4" t="n"/>
-      <c r="U14" s="4" t="n"/>
+      <c r="T14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U14" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V14" s="4" t="n"/>
       <c r="W14" s="4" t="n"/>
       <c r="X14" s="2" t="n"/>
@@ -2678,24 +3070,60 @@
       <c r="B15" s="23" t="n"/>
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="4" t="n"/>
-      <c r="E15" s="4" t="n"/>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="4" t="n"/>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I15" s="3" t="n"/>
-      <c r="J15" s="2" t="n"/>
-      <c r="K15" s="4" t="n"/>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L15" s="4" t="n"/>
-      <c r="M15" s="4" t="n"/>
+      <c r="M15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N15" s="4" t="n"/>
-      <c r="O15" s="4" t="n"/>
+      <c r="O15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P15" s="3" t="n"/>
       <c r="Q15" s="2" t="n"/>
-      <c r="R15" s="4" t="n"/>
+      <c r="R15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S15" s="4" t="n"/>
       <c r="T15" s="4" t="n"/>
       <c r="U15" s="4" t="n"/>
-      <c r="V15" s="4" t="n"/>
+      <c r="V15" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W15" s="4" t="n"/>
       <c r="X15" s="2" t="n"/>
       <c r="Y15" s="4" t="n"/>
@@ -2783,23 +3211,75 @@
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="4" t="n"/>
       <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="4" t="n"/>
-      <c r="I16" s="3" t="n"/>
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J16" s="2" t="n"/>
       <c r="K16" s="4" t="n"/>
-      <c r="L16" s="4" t="n"/>
-      <c r="M16" s="4" t="n"/>
-      <c r="N16" s="4" t="n"/>
+      <c r="L16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O16" s="4" t="n"/>
-      <c r="P16" s="3" t="n"/>
-      <c r="Q16" s="2" t="n"/>
-      <c r="R16" s="4" t="n"/>
+      <c r="P16" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q16" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S16" s="4" t="n"/>
-      <c r="T16" s="4" t="n"/>
-      <c r="U16" s="4" t="n"/>
-      <c r="V16" s="4" t="n"/>
+      <c r="T16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="V16" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W16" s="4" t="n"/>
       <c r="X16" s="2" t="n"/>
       <c r="Y16" s="4" t="n"/>
@@ -2886,23 +3366,59 @@
       <c r="B17" s="21" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="4" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G17" s="4" t="n"/>
-      <c r="H17" s="4" t="n"/>
+      <c r="H17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I17" s="3" t="n"/>
-      <c r="J17" s="2" t="n"/>
+      <c r="J17" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K17" s="4" t="n"/>
       <c r="L17" s="4" t="n"/>
       <c r="M17" s="4" t="n"/>
       <c r="N17" s="4" t="n"/>
-      <c r="O17" s="4" t="n"/>
-      <c r="P17" s="3" t="n"/>
+      <c r="O17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P17" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q17" s="2" t="n"/>
       <c r="R17" s="4" t="n"/>
-      <c r="S17" s="4" t="n"/>
-      <c r="T17" s="4" t="n"/>
-      <c r="U17" s="4" t="n"/>
+      <c r="S17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U17" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V17" s="4" t="n"/>
       <c r="W17" s="4" t="n"/>
       <c r="X17" s="2" t="n"/>
@@ -2990,24 +3506,72 @@
       </c>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="4" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G18" s="4" t="n"/>
-      <c r="H18" s="4" t="n"/>
-      <c r="I18" s="3" t="n"/>
+      <c r="H18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J18" s="2" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
+      <c r="K18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M18" s="4" t="n"/>
       <c r="N18" s="4" t="n"/>
       <c r="O18" s="4" t="n"/>
-      <c r="P18" s="3" t="n"/>
-      <c r="Q18" s="2" t="n"/>
-      <c r="R18" s="4" t="n"/>
-      <c r="S18" s="4" t="n"/>
+      <c r="P18" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q18" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T18" s="4" t="n"/>
-      <c r="U18" s="4" t="n"/>
-      <c r="V18" s="4" t="n"/>
+      <c r="U18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="V18" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W18" s="4" t="n"/>
       <c r="X18" s="2" t="n"/>
       <c r="Y18" s="4" t="n"/>
@@ -3094,29 +3658,77 @@
       <c r="B19" s="23" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I19" s="3" t="n"/>
-      <c r="J19" s="2" t="n"/>
+      <c r="J19" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
+      <c r="L19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M19" s="4" t="n"/>
       <c r="N19" s="4" t="n"/>
-      <c r="O19" s="4" t="n"/>
-      <c r="P19" s="3" t="n"/>
-      <c r="Q19" s="2" t="n"/>
+      <c r="O19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P19" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q19" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R19" s="4" t="n"/>
-      <c r="S19" s="4" t="n"/>
-      <c r="T19" s="4" t="n"/>
+      <c r="S19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U19" s="4" t="n"/>
-      <c r="V19" s="4" t="n"/>
+      <c r="V19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W19" s="4" t="n"/>
       <c r="X19" s="2" t="n"/>
       <c r="Y19" s="4" t="n"/>
       <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="n"/>
+      <c r="AA19" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AB19" s="4" t="n"/>
       <c r="AC19" s="4" t="n"/>
       <c r="AD19" s="3" t="n"/>
@@ -3202,19 +3814,39 @@
       <c r="F20" s="4" t="n"/>
       <c r="G20" s="4" t="n"/>
       <c r="H20" s="4" t="n"/>
-      <c r="I20" s="3" t="n"/>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J20" s="2" t="n"/>
       <c r="K20" s="4" t="n"/>
       <c r="L20" s="4" t="n"/>
       <c r="M20" s="4" t="n"/>
-      <c r="N20" s="4" t="n"/>
-      <c r="O20" s="4" t="n"/>
+      <c r="N20" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O20" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P20" s="3" t="n"/>
-      <c r="Q20" s="2" t="n"/>
+      <c r="Q20" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R20" s="4" t="n"/>
       <c r="S20" s="4" t="n"/>
       <c r="T20" s="4" t="n"/>
-      <c r="U20" s="4" t="n"/>
+      <c r="U20" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V20" s="4" t="n"/>
       <c r="W20" s="4" t="n"/>
       <c r="X20" s="2" t="n"/>
@@ -3302,24 +3934,52 @@
       <c r="B21" s="21" t="n"/>
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G21" s="4" t="n"/>
-      <c r="H21" s="4" t="n"/>
+      <c r="H21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I21" s="3" t="n"/>
       <c r="J21" s="2" t="n"/>
       <c r="K21" s="4" t="n"/>
       <c r="L21" s="4" t="n"/>
       <c r="M21" s="4" t="n"/>
-      <c r="N21" s="4" t="n"/>
+      <c r="N21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O21" s="4" t="n"/>
       <c r="P21" s="3" t="n"/>
       <c r="Q21" s="2" t="n"/>
-      <c r="R21" s="4" t="n"/>
+      <c r="R21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S21" s="4" t="n"/>
-      <c r="T21" s="4" t="n"/>
+      <c r="T21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U21" s="4" t="n"/>
-      <c r="V21" s="4" t="n"/>
+      <c r="V21" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W21" s="4" t="n"/>
       <c r="X21" s="2" t="n"/>
       <c r="Y21" s="4" t="n"/>
@@ -3407,23 +4067,59 @@
       <c r="C22" s="4" t="n"/>
       <c r="D22" s="4" t="n"/>
       <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G22" s="4" t="n"/>
       <c r="H22" s="4" t="n"/>
-      <c r="I22" s="3" t="n"/>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J22" s="2" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M22" s="4" t="n"/>
-      <c r="N22" s="4" t="n"/>
+      <c r="N22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O22" s="4" t="n"/>
       <c r="P22" s="3" t="n"/>
-      <c r="Q22" s="2" t="n"/>
-      <c r="R22" s="4" t="n"/>
-      <c r="S22" s="4" t="n"/>
+      <c r="Q22" s="2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T22" s="4" t="n"/>
       <c r="U22" s="4" t="n"/>
-      <c r="V22" s="4" t="n"/>
+      <c r="V22" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W22" s="4" t="n"/>
       <c r="X22" s="2" t="n"/>
       <c r="Y22" s="4" t="n"/>
@@ -3511,7 +4207,11 @@
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="4" t="n"/>
       <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G23" s="4" t="n"/>
       <c r="H23" s="4" t="n"/>
       <c r="I23" s="3" t="n"/>
@@ -3519,15 +4219,27 @@
       <c r="K23" s="4" t="n"/>
       <c r="L23" s="4" t="n"/>
       <c r="M23" s="4" t="n"/>
-      <c r="N23" s="4" t="n"/>
+      <c r="N23" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O23" s="4" t="n"/>
       <c r="P23" s="3" t="n"/>
       <c r="Q23" s="2" t="n"/>
       <c r="R23" s="4" t="n"/>
-      <c r="S23" s="4" t="n"/>
+      <c r="S23" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T23" s="4" t="n"/>
       <c r="U23" s="4" t="n"/>
-      <c r="V23" s="4" t="n"/>
+      <c r="V23" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W23" s="4" t="n"/>
       <c r="X23" s="2" t="n"/>
       <c r="Y23" s="4" t="n"/>
@@ -3618,9 +4330,17 @@
       <c r="F24" s="4" t="n"/>
       <c r="G24" s="4" t="n"/>
       <c r="H24" s="4" t="n"/>
-      <c r="I24" s="3" t="n"/>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J24" s="2" t="n"/>
-      <c r="K24" s="4" t="n"/>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L24" s="4" t="n"/>
       <c r="M24" s="4" t="n"/>
       <c r="N24" s="4" t="n"/>
@@ -3635,7 +4355,11 @@
       <c r="W24" s="4" t="n"/>
       <c r="X24" s="2" t="n"/>
       <c r="Y24" s="4" t="n"/>
-      <c r="Z24" s="4" t="n"/>
+      <c r="Z24" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA24" s="4" t="n"/>
       <c r="AB24" s="4" t="n"/>
       <c r="AC24" s="4" t="n"/>
@@ -3829,7 +4553,11 @@
       <c r="I26" s="3" t="n"/>
       <c r="J26" s="2" t="n"/>
       <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
+      <c r="L26" s="4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M26" s="4" t="n"/>
       <c r="N26" s="4" t="n"/>
       <c r="O26" s="4" t="n"/>
@@ -3938,11 +4666,7 @@
       <c r="N27" s="6" t="n"/>
       <c r="O27" s="6" t="n"/>
       <c r="P27" s="7" t="n"/>
-      <c r="Q27" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Q27" s="5" t="n"/>
       <c r="R27" s="6" t="n"/>
       <c r="S27" s="6" t="n"/>
       <c r="T27" s="6" t="n"/>
@@ -4428,28 +5152,28 @@
     </row>
     <row r="30">
       <c r="B30" s="1" t="n"/>
-      <c r="C30" s="32" t="inlineStr">
+      <c r="C30" s="38" t="inlineStr">
         <is>
           <t>data rozpoczęcia, poniedziałek -&gt;</t>
         </is>
       </c>
-      <c r="D30" s="33" t="n"/>
-      <c r="E30" s="33" t="n"/>
-      <c r="F30" s="33" t="n"/>
-      <c r="G30" s="33" t="n"/>
-      <c r="H30" s="33" t="n"/>
-      <c r="I30" s="33" t="n"/>
-      <c r="J30" s="33" t="n"/>
-      <c r="K30" s="33" t="n"/>
-      <c r="L30" s="33" t="n"/>
-      <c r="M30" s="33" t="n"/>
-      <c r="N30" s="34" t="n">
+      <c r="D30" s="36" t="n"/>
+      <c r="E30" s="36" t="n"/>
+      <c r="F30" s="36" t="n"/>
+      <c r="G30" s="36" t="n"/>
+      <c r="H30" s="36" t="n"/>
+      <c r="I30" s="36" t="n"/>
+      <c r="J30" s="36" t="n"/>
+      <c r="K30" s="36" t="n"/>
+      <c r="L30" s="36" t="n"/>
+      <c r="M30" s="36" t="n"/>
+      <c r="N30" s="35" t="n">
         <v>44949</v>
       </c>
-      <c r="O30" s="33" t="n"/>
-      <c r="P30" s="33" t="n"/>
-      <c r="Q30" s="33" t="n"/>
-      <c r="R30" s="35" t="n"/>
+      <c r="O30" s="36" t="n"/>
+      <c r="P30" s="36" t="n"/>
+      <c r="Q30" s="36" t="n"/>
+      <c r="R30" s="37" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="1" t="n"/>
@@ -4470,7 +5194,6 @@
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="CB2:CH2"/>
-    <mergeCell ref="AS2:AY2"/>
     <mergeCell ref="BN2:BT2"/>
     <mergeCell ref="AL2:AR2"/>
     <mergeCell ref="CI2:CO2"/>
@@ -4478,11 +5201,12 @@
     <mergeCell ref="CP2:CV2"/>
     <mergeCell ref="N30:R30"/>
     <mergeCell ref="C30:M30"/>
+    <mergeCell ref="J2:P2"/>
     <mergeCell ref="B1:CV1"/>
     <mergeCell ref="Q2:W2"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="X2:AD2"/>
-    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="AS2:AY2"/>
     <mergeCell ref="AE2:AK2"/>
     <mergeCell ref="AZ2:BF2"/>
     <mergeCell ref="BG2:BM2"/>

</xml_diff>